<commit_message>
trying to fix fe nigga
</commit_message>
<xml_diff>
--- a/data/Menus.xlsx
+++ b/data/Menus.xlsx
@@ -652,7 +652,7 @@
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="right" vertical="bottom"/>
+      <alignment horizontal="right" readingOrder="0" vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
@@ -889,7 +889,7 @@
     </row>
     <row r="2">
       <c r="A2" s="2">
-        <v>1.0</v>
+        <v>408.0</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>3</v>
@@ -900,7 +900,7 @@
     </row>
     <row r="3">
       <c r="A3" s="2">
-        <v>2.0</v>
+        <v>409.0</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>5</v>
@@ -911,7 +911,7 @@
     </row>
     <row r="4">
       <c r="A4" s="2">
-        <v>3.0</v>
+        <v>410.0</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>7</v>
@@ -922,7 +922,7 @@
     </row>
     <row r="5">
       <c r="A5" s="2">
-        <v>4.0</v>
+        <v>411.0</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>9</v>
@@ -933,7 +933,7 @@
     </row>
     <row r="6">
       <c r="A6" s="2">
-        <v>5.0</v>
+        <v>412.0</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>11</v>
@@ -944,7 +944,7 @@
     </row>
     <row r="7">
       <c r="A7" s="2">
-        <v>6.0</v>
+        <v>413.0</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>13</v>
@@ -955,7 +955,7 @@
     </row>
     <row r="8">
       <c r="A8" s="2">
-        <v>7.0</v>
+        <v>414.0</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>15</v>
@@ -966,7 +966,7 @@
     </row>
     <row r="9">
       <c r="A9" s="2">
-        <v>8.0</v>
+        <v>415.0</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>17</v>
@@ -977,7 +977,7 @@
     </row>
     <row r="10">
       <c r="A10" s="2">
-        <v>9.0</v>
+        <v>416.0</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>19</v>
@@ -988,7 +988,7 @@
     </row>
     <row r="11">
       <c r="A11" s="2">
-        <v>10.0</v>
+        <v>417.0</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>21</v>
@@ -999,7 +999,7 @@
     </row>
     <row r="12">
       <c r="A12" s="2">
-        <v>11.0</v>
+        <v>418.0</v>
       </c>
       <c r="B12" s="3" t="s">
         <v>23</v>
@@ -1010,7 +1010,7 @@
     </row>
     <row r="13">
       <c r="A13" s="2">
-        <v>12.0</v>
+        <v>419.0</v>
       </c>
       <c r="B13" s="3" t="s">
         <v>25</v>
@@ -1021,7 +1021,7 @@
     </row>
     <row r="14">
       <c r="A14" s="2">
-        <v>13.0</v>
+        <v>420.0</v>
       </c>
       <c r="B14" s="3" t="s">
         <v>27</v>
@@ -1032,7 +1032,7 @@
     </row>
     <row r="15">
       <c r="A15" s="2">
-        <v>14.0</v>
+        <v>421.0</v>
       </c>
       <c r="B15" s="3" t="s">
         <v>29</v>
@@ -1043,7 +1043,7 @@
     </row>
     <row r="16">
       <c r="A16" s="2">
-        <v>15.0</v>
+        <v>422.0</v>
       </c>
       <c r="B16" s="3" t="s">
         <v>31</v>
@@ -1054,7 +1054,7 @@
     </row>
     <row r="17">
       <c r="A17" s="2">
-        <v>16.0</v>
+        <v>423.0</v>
       </c>
       <c r="B17" s="3" t="s">
         <v>33</v>
@@ -1065,7 +1065,7 @@
     </row>
     <row r="18">
       <c r="A18" s="2">
-        <v>17.0</v>
+        <v>424.0</v>
       </c>
       <c r="B18" s="3" t="s">
         <v>35</v>
@@ -1076,7 +1076,7 @@
     </row>
     <row r="19">
       <c r="A19" s="2">
-        <v>18.0</v>
+        <v>425.0</v>
       </c>
       <c r="B19" s="3" t="s">
         <v>37</v>
@@ -1087,7 +1087,7 @@
     </row>
     <row r="20">
       <c r="A20" s="2">
-        <v>19.0</v>
+        <v>426.0</v>
       </c>
       <c r="B20" s="3" t="s">
         <v>39</v>
@@ -1098,7 +1098,7 @@
     </row>
     <row r="21">
       <c r="A21" s="2">
-        <v>20.0</v>
+        <v>427.0</v>
       </c>
       <c r="B21" s="3" t="s">
         <v>41</v>
@@ -1109,7 +1109,7 @@
     </row>
     <row r="22">
       <c r="A22" s="2">
-        <v>21.0</v>
+        <v>428.0</v>
       </c>
       <c r="B22" s="3" t="s">
         <v>43</v>
@@ -1120,7 +1120,7 @@
     </row>
     <row r="23">
       <c r="A23" s="2">
-        <v>22.0</v>
+        <v>429.0</v>
       </c>
       <c r="B23" s="3" t="s">
         <v>45</v>
@@ -1131,7 +1131,7 @@
     </row>
     <row r="24">
       <c r="A24" s="2">
-        <v>23.0</v>
+        <v>430.0</v>
       </c>
       <c r="B24" s="3" t="s">
         <v>47</v>
@@ -1142,7 +1142,7 @@
     </row>
     <row r="25">
       <c r="A25" s="2">
-        <v>24.0</v>
+        <v>431.0</v>
       </c>
       <c r="B25" s="3" t="s">
         <v>49</v>
@@ -1153,7 +1153,7 @@
     </row>
     <row r="26">
       <c r="A26" s="2">
-        <v>25.0</v>
+        <v>432.0</v>
       </c>
       <c r="B26" s="3" t="s">
         <v>51</v>
@@ -1164,7 +1164,7 @@
     </row>
     <row r="27">
       <c r="A27" s="2">
-        <v>26.0</v>
+        <v>433.0</v>
       </c>
       <c r="B27" s="3" t="s">
         <v>53</v>
@@ -1175,7 +1175,7 @@
     </row>
     <row r="28">
       <c r="A28" s="2">
-        <v>27.0</v>
+        <v>434.0</v>
       </c>
       <c r="B28" s="3" t="s">
         <v>55</v>
@@ -1186,7 +1186,7 @@
     </row>
     <row r="29">
       <c r="A29" s="2">
-        <v>28.0</v>
+        <v>435.0</v>
       </c>
       <c r="B29" s="3" t="s">
         <v>57</v>
@@ -1197,7 +1197,7 @@
     </row>
     <row r="30">
       <c r="A30" s="2">
-        <v>29.0</v>
+        <v>436.0</v>
       </c>
       <c r="B30" s="3" t="s">
         <v>59</v>
@@ -1208,7 +1208,7 @@
     </row>
     <row r="31">
       <c r="A31" s="2">
-        <v>30.0</v>
+        <v>437.0</v>
       </c>
       <c r="B31" s="3" t="s">
         <v>61</v>
@@ -1219,7 +1219,7 @@
     </row>
     <row r="32">
       <c r="A32" s="2">
-        <v>31.0</v>
+        <v>438.0</v>
       </c>
       <c r="B32" s="3" t="s">
         <v>63</v>
@@ -1230,7 +1230,7 @@
     </row>
     <row r="33">
       <c r="A33" s="2">
-        <v>32.0</v>
+        <v>439.0</v>
       </c>
       <c r="B33" s="3" t="s">
         <v>65</v>
@@ -1241,7 +1241,7 @@
     </row>
     <row r="34">
       <c r="A34" s="2">
-        <v>33.0</v>
+        <v>440.0</v>
       </c>
       <c r="B34" s="3" t="s">
         <v>67</v>
@@ -1252,7 +1252,7 @@
     </row>
     <row r="35">
       <c r="A35" s="2">
-        <v>34.0</v>
+        <v>441.0</v>
       </c>
       <c r="B35" s="3" t="s">
         <v>65</v>
@@ -1263,7 +1263,7 @@
     </row>
     <row r="36">
       <c r="A36" s="2">
-        <v>35.0</v>
+        <v>442.0</v>
       </c>
       <c r="B36" s="3" t="s">
         <v>70</v>
@@ -1274,7 +1274,7 @@
     </row>
     <row r="37">
       <c r="A37" s="2">
-        <v>36.0</v>
+        <v>443.0</v>
       </c>
       <c r="B37" s="3" t="s">
         <v>72</v>
@@ -1285,7 +1285,7 @@
     </row>
     <row r="38">
       <c r="A38" s="2">
-        <v>37.0</v>
+        <v>444.0</v>
       </c>
       <c r="B38" s="3" t="s">
         <v>74</v>
@@ -1296,7 +1296,7 @@
     </row>
     <row r="39">
       <c r="A39" s="2">
-        <v>38.0</v>
+        <v>445.0</v>
       </c>
       <c r="B39" s="3" t="s">
         <v>76</v>
@@ -1307,7 +1307,7 @@
     </row>
     <row r="40">
       <c r="A40" s="2">
-        <v>39.0</v>
+        <v>446.0</v>
       </c>
       <c r="B40" s="3" t="s">
         <v>78</v>
@@ -1318,7 +1318,7 @@
     </row>
     <row r="41">
       <c r="A41" s="2">
-        <v>40.0</v>
+        <v>447.0</v>
       </c>
       <c r="B41" s="3" t="s">
         <v>80</v>
@@ -1329,7 +1329,7 @@
     </row>
     <row r="42">
       <c r="A42" s="2">
-        <v>41.0</v>
+        <v>448.0</v>
       </c>
       <c r="B42" s="3" t="s">
         <v>82</v>
@@ -1340,7 +1340,7 @@
     </row>
     <row r="43">
       <c r="A43" s="2">
-        <v>42.0</v>
+        <v>449.0</v>
       </c>
       <c r="B43" s="3" t="s">
         <v>84</v>
@@ -1351,7 +1351,7 @@
     </row>
     <row r="44">
       <c r="A44" s="2">
-        <v>43.0</v>
+        <v>450.0</v>
       </c>
       <c r="B44" s="3" t="s">
         <v>86</v>
@@ -1362,7 +1362,7 @@
     </row>
     <row r="45">
       <c r="A45" s="2">
-        <v>44.0</v>
+        <v>451.0</v>
       </c>
       <c r="B45" s="3" t="s">
         <v>88</v>
@@ -1373,7 +1373,7 @@
     </row>
     <row r="46">
       <c r="A46" s="2">
-        <v>45.0</v>
+        <v>452.0</v>
       </c>
       <c r="B46" s="3" t="s">
         <v>90</v>
@@ -1384,7 +1384,7 @@
     </row>
     <row r="47">
       <c r="A47" s="2">
-        <v>46.0</v>
+        <v>453.0</v>
       </c>
       <c r="B47" s="3" t="s">
         <v>92</v>
@@ -1395,7 +1395,7 @@
     </row>
     <row r="48">
       <c r="A48" s="2">
-        <v>47.0</v>
+        <v>454.0</v>
       </c>
       <c r="B48" s="3" t="s">
         <v>94</v>
@@ -1406,7 +1406,7 @@
     </row>
     <row r="49">
       <c r="A49" s="2">
-        <v>48.0</v>
+        <v>455.0</v>
       </c>
       <c r="B49" s="3" t="s">
         <v>96</v>
@@ -1417,7 +1417,7 @@
     </row>
     <row r="50">
       <c r="A50" s="2">
-        <v>49.0</v>
+        <v>456.0</v>
       </c>
       <c r="B50" s="3" t="s">
         <v>98</v>
@@ -1428,7 +1428,7 @@
     </row>
     <row r="51">
       <c r="A51" s="2">
-        <v>50.0</v>
+        <v>457.0</v>
       </c>
       <c r="B51" s="3" t="s">
         <v>100</v>
@@ -1439,7 +1439,7 @@
     </row>
     <row r="52">
       <c r="A52" s="2">
-        <v>51.0</v>
+        <v>458.0</v>
       </c>
       <c r="B52" s="3" t="s">
         <v>102</v>
@@ -1450,7 +1450,7 @@
     </row>
     <row r="53">
       <c r="A53" s="2">
-        <v>52.0</v>
+        <v>459.0</v>
       </c>
       <c r="B53" s="3" t="s">
         <v>104</v>
@@ -1461,7 +1461,7 @@
     </row>
     <row r="54">
       <c r="A54" s="2">
-        <v>53.0</v>
+        <v>460.0</v>
       </c>
       <c r="B54" s="3" t="s">
         <v>106</v>
@@ -1472,7 +1472,7 @@
     </row>
     <row r="55">
       <c r="A55" s="2">
-        <v>54.0</v>
+        <v>461.0</v>
       </c>
       <c r="B55" s="3" t="s">
         <v>108</v>
@@ -1483,7 +1483,7 @@
     </row>
     <row r="56">
       <c r="A56" s="2">
-        <v>55.0</v>
+        <v>462.0</v>
       </c>
       <c r="B56" s="3" t="s">
         <v>110</v>
@@ -1494,7 +1494,7 @@
     </row>
     <row r="57">
       <c r="A57" s="2">
-        <v>56.0</v>
+        <v>463.0</v>
       </c>
       <c r="B57" s="3" t="s">
         <v>112</v>
@@ -1505,7 +1505,7 @@
     </row>
     <row r="58">
       <c r="A58" s="2">
-        <v>57.0</v>
+        <v>464.0</v>
       </c>
       <c r="B58" s="3" t="s">
         <v>114</v>
@@ -1516,7 +1516,7 @@
     </row>
     <row r="59">
       <c r="A59" s="2">
-        <v>58.0</v>
+        <v>465.0</v>
       </c>
       <c r="B59" s="3" t="s">
         <v>116</v>
@@ -1527,7 +1527,7 @@
     </row>
     <row r="60">
       <c r="A60" s="2">
-        <v>59.0</v>
+        <v>466.0</v>
       </c>
       <c r="B60" s="3" t="s">
         <v>118</v>
@@ -1538,7 +1538,7 @@
     </row>
     <row r="61">
       <c r="A61" s="2">
-        <v>60.0</v>
+        <v>467.0</v>
       </c>
       <c r="B61" s="3" t="s">
         <v>120</v>
@@ -1549,7 +1549,7 @@
     </row>
     <row r="62">
       <c r="A62" s="2">
-        <v>61.0</v>
+        <v>468.0</v>
       </c>
       <c r="B62" s="3" t="s">
         <v>122</v>
@@ -1560,7 +1560,7 @@
     </row>
     <row r="63">
       <c r="A63" s="2">
-        <v>62.0</v>
+        <v>469.0</v>
       </c>
       <c r="B63" s="3" t="s">
         <v>124</v>
@@ -1571,7 +1571,7 @@
     </row>
     <row r="64">
       <c r="A64" s="2">
-        <v>63.0</v>
+        <v>470.0</v>
       </c>
       <c r="B64" s="3" t="s">
         <v>126</v>
@@ -1582,7 +1582,7 @@
     </row>
     <row r="65">
       <c r="A65" s="2">
-        <v>64.0</v>
+        <v>471.0</v>
       </c>
       <c r="B65" s="3" t="s">
         <v>128</v>
@@ -1593,7 +1593,7 @@
     </row>
     <row r="66">
       <c r="A66" s="2">
-        <v>65.0</v>
+        <v>472.0</v>
       </c>
       <c r="B66" s="3" t="s">
         <v>130</v>
@@ -1604,7 +1604,7 @@
     </row>
     <row r="67">
       <c r="A67" s="2">
-        <v>66.0</v>
+        <v>473.0</v>
       </c>
       <c r="B67" s="3" t="s">
         <v>132</v>
@@ -1615,7 +1615,7 @@
     </row>
     <row r="68">
       <c r="A68" s="2">
-        <v>67.0</v>
+        <v>474.0</v>
       </c>
       <c r="B68" s="3" t="s">
         <v>134</v>
@@ -1626,7 +1626,7 @@
     </row>
     <row r="69">
       <c r="A69" s="2">
-        <v>68.0</v>
+        <v>475.0</v>
       </c>
       <c r="B69" s="3" t="s">
         <v>136</v>
@@ -1637,7 +1637,7 @@
     </row>
     <row r="70">
       <c r="A70" s="2">
-        <v>69.0</v>
+        <v>476.0</v>
       </c>
       <c r="B70" s="3" t="s">
         <v>138</v>
@@ -1648,7 +1648,7 @@
     </row>
     <row r="71">
       <c r="A71" s="2">
-        <v>70.0</v>
+        <v>477.0</v>
       </c>
       <c r="B71" s="3" t="s">
         <v>140</v>
@@ -1659,7 +1659,7 @@
     </row>
     <row r="72">
       <c r="A72" s="2">
-        <v>71.0</v>
+        <v>478.0</v>
       </c>
       <c r="B72" s="3" t="s">
         <v>142</v>
@@ -1670,7 +1670,7 @@
     </row>
     <row r="73">
       <c r="A73" s="2">
-        <v>72.0</v>
+        <v>479.0</v>
       </c>
       <c r="B73" s="3" t="s">
         <v>144</v>
@@ -1681,7 +1681,7 @@
     </row>
     <row r="74">
       <c r="A74" s="2">
-        <v>73.0</v>
+        <v>480.0</v>
       </c>
       <c r="B74" s="3" t="s">
         <v>146</v>
@@ -1692,7 +1692,7 @@
     </row>
     <row r="75">
       <c r="A75" s="2">
-        <v>74.0</v>
+        <v>481.0</v>
       </c>
       <c r="B75" s="3" t="s">
         <v>148</v>
@@ -1703,7 +1703,7 @@
     </row>
     <row r="76">
       <c r="A76" s="2">
-        <v>75.0</v>
+        <v>482.0</v>
       </c>
       <c r="B76" s="3" t="s">
         <v>150</v>
@@ -1714,7 +1714,7 @@
     </row>
     <row r="77">
       <c r="A77" s="2">
-        <v>76.0</v>
+        <v>483.0</v>
       </c>
       <c r="B77" s="3" t="s">
         <v>152</v>
@@ -1725,7 +1725,7 @@
     </row>
     <row r="78">
       <c r="A78" s="2">
-        <v>77.0</v>
+        <v>484.0</v>
       </c>
       <c r="B78" s="3" t="s">
         <v>154</v>
@@ -1736,7 +1736,7 @@
     </row>
     <row r="79">
       <c r="A79" s="2">
-        <v>78.0</v>
+        <v>485.0</v>
       </c>
       <c r="B79" s="3" t="s">
         <v>156</v>
@@ -1747,7 +1747,7 @@
     </row>
     <row r="80">
       <c r="A80" s="2">
-        <v>79.0</v>
+        <v>486.0</v>
       </c>
       <c r="B80" s="3" t="s">
         <v>158</v>
@@ -1758,7 +1758,7 @@
     </row>
     <row r="81">
       <c r="A81" s="2">
-        <v>80.0</v>
+        <v>487.0</v>
       </c>
       <c r="B81" s="3" t="s">
         <v>160</v>
@@ -1769,7 +1769,7 @@
     </row>
     <row r="82">
       <c r="A82" s="2">
-        <v>81.0</v>
+        <v>488.0</v>
       </c>
       <c r="B82" s="3" t="s">
         <v>162</v>
@@ -1780,7 +1780,7 @@
     </row>
     <row r="83">
       <c r="A83" s="2">
-        <v>82.0</v>
+        <v>489.0</v>
       </c>
       <c r="B83" s="3" t="s">
         <v>164</v>
@@ -1791,7 +1791,7 @@
     </row>
     <row r="84">
       <c r="A84" s="2">
-        <v>83.0</v>
+        <v>490.0</v>
       </c>
       <c r="B84" s="3" t="s">
         <v>166</v>
@@ -1802,7 +1802,7 @@
     </row>
     <row r="85">
       <c r="A85" s="2">
-        <v>84.0</v>
+        <v>491.0</v>
       </c>
       <c r="B85" s="3" t="s">
         <v>168</v>
@@ -1813,7 +1813,7 @@
     </row>
     <row r="86">
       <c r="A86" s="2">
-        <v>85.0</v>
+        <v>492.0</v>
       </c>
       <c r="B86" s="3" t="s">
         <v>170</v>
@@ -1824,7 +1824,7 @@
     </row>
     <row r="87">
       <c r="A87" s="2">
-        <v>86.0</v>
+        <v>493.0</v>
       </c>
       <c r="B87" s="3" t="s">
         <v>172</v>
@@ -1835,7 +1835,7 @@
     </row>
     <row r="88">
       <c r="A88" s="2">
-        <v>87.0</v>
+        <v>494.0</v>
       </c>
       <c r="B88" s="3" t="s">
         <v>174</v>
@@ -1846,7 +1846,7 @@
     </row>
     <row r="89">
       <c r="A89" s="2">
-        <v>88.0</v>
+        <v>495.0</v>
       </c>
       <c r="B89" s="3" t="s">
         <v>176</v>
@@ -1857,7 +1857,7 @@
     </row>
     <row r="90">
       <c r="A90" s="2">
-        <v>89.0</v>
+        <v>496.0</v>
       </c>
       <c r="B90" s="3" t="s">
         <v>178</v>
@@ -1868,7 +1868,7 @@
     </row>
     <row r="91">
       <c r="A91" s="2">
-        <v>90.0</v>
+        <v>497.0</v>
       </c>
       <c r="B91" s="3" t="s">
         <v>180</v>
@@ -1879,7 +1879,7 @@
     </row>
     <row r="92">
       <c r="A92" s="2">
-        <v>91.0</v>
+        <v>498.0</v>
       </c>
       <c r="B92" s="3" t="s">
         <v>182</v>
@@ -1890,7 +1890,7 @@
     </row>
     <row r="93">
       <c r="A93" s="2">
-        <v>92.0</v>
+        <v>499.0</v>
       </c>
       <c r="B93" s="3" t="s">
         <v>184</v>
@@ -1901,7 +1901,7 @@
     </row>
     <row r="94">
       <c r="A94" s="2">
-        <v>93.0</v>
+        <v>500.0</v>
       </c>
       <c r="B94" s="3" t="s">
         <v>186</v>
@@ -1912,7 +1912,7 @@
     </row>
     <row r="95">
       <c r="A95" s="2">
-        <v>94.0</v>
+        <v>501.0</v>
       </c>
       <c r="B95" s="3" t="s">
         <v>188</v>
@@ -1923,7 +1923,7 @@
     </row>
     <row r="96">
       <c r="A96" s="2">
-        <v>95.0</v>
+        <v>502.0</v>
       </c>
       <c r="B96" s="3" t="s">
         <v>190</v>
@@ -1934,7 +1934,7 @@
     </row>
     <row r="97">
       <c r="A97" s="2">
-        <v>96.0</v>
+        <v>503.0</v>
       </c>
       <c r="B97" s="3" t="s">
         <v>192</v>
@@ -1945,7 +1945,7 @@
     </row>
     <row r="98">
       <c r="A98" s="2">
-        <v>97.0</v>
+        <v>504.0</v>
       </c>
       <c r="B98" s="3" t="s">
         <v>194</v>
@@ -1956,7 +1956,7 @@
     </row>
     <row r="99">
       <c r="A99" s="2">
-        <v>98.0</v>
+        <v>505.0</v>
       </c>
       <c r="B99" s="3" t="s">
         <v>196</v>
@@ -1967,7 +1967,7 @@
     </row>
     <row r="100">
       <c r="A100" s="2">
-        <v>99.0</v>
+        <v>506.0</v>
       </c>
       <c r="B100" s="3" t="s">
         <v>198</v>

</xml_diff>